<commit_message>
Création des clips de maps dans le dernier frame (À RETIRER DÈS QUE LA MAP EST TRACÉE)
</commit_message>
<xml_diff>
--- a/Epopee/Documentation/Map.xlsx
+++ b/Epopee/Documentation/Map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Documents\Projets\Controle Qualité\Epopee\Croquis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STGF1431024\_preAlpha\Epopee\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14295"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <r>
       <t xml:space="preserve">Vilage 1
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>Forêt perdue 1</t>
-  </si>
-  <si>
-    <t>Forêt perdue</t>
   </si>
   <si>
     <t>Forêt perdue 2</t>
@@ -275,11 +272,23 @@
       <t>Boss</t>
     </r>
   </si>
+  <si>
+    <t>Forêt perdue 5</t>
+  </si>
+  <si>
+    <t>Forêt perdue 6</t>
+  </si>
+  <si>
+    <t>Forêt perdue 7</t>
+  </si>
+  <si>
+    <t>Forêt perdue 8</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -835,7 +844,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.42578125" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -861,7 +870,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -877,17 +886,17 @@
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="13" t="s">
         <v>16</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>17</v>
       </c>
       <c r="J3" s="2"/>
     </row>
@@ -902,17 +911,17 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>3</v>
@@ -922,7 +931,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -930,21 +939,21 @@
     <row r="6" spans="1:10" ht="75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -952,25 +961,25 @@
     <row r="7" spans="1:10" ht="75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="10" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -979,13 +988,13 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -996,16 +1005,16 @@
     <row r="9" spans="1:10" ht="75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>10</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1016,12 +1025,12 @@
     <row r="10" spans="1:10" ht="75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>

</xml_diff>